<commit_message>
added flight ensemble classifier
</commit_message>
<xml_diff>
--- a/Datasets/locations_with_id.xlsx
+++ b/Datasets/locations_with_id.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26306"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26330"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F000D773-01C1-40DA-8CC4-7C7386D896DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E5C146C-36D3-4CD0-B9D3-6C1078367AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3736,8 +3736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A285" workbookViewId="0">
-      <selection activeCell="E300" sqref="E300"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="E133" sqref="E133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -8149,11 +8149,11 @@
       <c r="C133" s="1">
         <v>188</v>
       </c>
-      <c r="D133" s="1">
-        <v>43.397199999999998</v>
-      </c>
-      <c r="E133" s="1">
-        <v>-80.311400000000006</v>
+      <c r="D133" s="17">
+        <v>52.205275999999998</v>
+      </c>
+      <c r="E133" s="17">
+        <v>0.119167</v>
       </c>
       <c r="F133" s="1">
         <v>129920</v>

</xml_diff>